<commit_message>
National Schematron schemas: Corrected nemSch_e182 and nemSch_e187. Updated element names for eInjury.03 and eInjury.04 per XSD change.
</commit_message>
<xml_diff>
--- a/Schematron/documentation/Schematron_3.4.0_3.5.0_Comparison.xlsx
+++ b/Schematron/documentation/Schematron_3.4.0_3.5.0_Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis\Schematron\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAD2497-E7E2-4CA6-9AA0-EC3EA29B3422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20676D51-0773-42CF-81B1-CC9508344358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EFB0DDD4-CF85-4C10-9AFB-9B88D9ECAAEF}"/>
   </bookViews>
@@ -1159,9 +1159,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>3.5.0.211008CP3</t>
-  </si>
-  <si>
     <t>This rule enforces no constraints on the combination of xsi:nil, Not Value, and Pertinent Negative attributes on Custom Data Element Result.</t>
   </si>
   <si>
@@ -1495,15 +1492,9 @@
     <t>Trauma Center Criteria should only be recorded when Possible Injury is "Yes".</t>
   </si>
   <si>
-    <t>Trauma Triage Criteria (Steps 1 and 2) should only be recorded when Possible Injury is "Yes".</t>
-  </si>
-  <si>
     <t>Vehicular, Pedestrian or Other Injury Risk Factor should only be recorded when Possible Injury is "Yes".</t>
   </si>
   <si>
-    <t>Trauma Triage Criteria (Steps 3 and 4) should only be recorded when Possible Injury is "Yes".</t>
-  </si>
-  <si>
     <t>Cardiac Arrest Etiology should be recorded when Cardiac Arrest is "Yes...".</t>
   </si>
   <si>
@@ -1813,12 +1804,6 @@
     <t>Level of Care Provided per Protocol should be recorded (with a value other than "No Care Provided") when Patient Evaluation/Care is "Patient Evaluated and Care Provided".</t>
   </si>
   <si>
-    <t>National Schematron Rules Comparison for DEMDataSet - June 23, 2022</t>
-  </si>
-  <si>
-    <t>National Schematron Rules Comparison for EMSDataSet - June 23, 2022</t>
-  </si>
-  <si>
     <t>Unit En Route Date/Time should be recorded unless Incident/Patient Disposition is "Canceled (Prior to Arrival At Scene)".</t>
   </si>
   <si>
@@ -1916,6 +1901,21 @@
   </si>
   <si>
     <t>Unit En Route Date/Time should be recorded unless Unit Disposition is "Cancelled Prior to Arrival at Scene".</t>
+  </si>
+  <si>
+    <t>Trauma Triage Criteria (High Risk for Serious Injury) should only be recorded when Possible Injury is "Yes".</t>
+  </si>
+  <si>
+    <t>Trauma Triage Criteria (Moderate Risk for Serious Injury) should only be recorded when Possible Injury is "Yes".</t>
+  </si>
+  <si>
+    <t>National Schematron Rules Comparison for EMSDataSet - March 17, 2023</t>
+  </si>
+  <si>
+    <t>3.5.0.230317CP4</t>
+  </si>
+  <si>
+    <t>National Schematron Rules Comparison for DEMDataSet - March 17, 2023</t>
   </si>
 </sst>
 </file>
@@ -1959,7 +1959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1969,9 +1969,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2521,27 +2518,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2574,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2583,7 +2580,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2594,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -2603,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -2614,7 +2611,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -2623,7 +2620,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2634,7 +2631,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -2643,7 +2640,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2654,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -2663,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2674,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2696,7 +2693,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>21</v>
@@ -2705,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2716,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>22</v>
@@ -2725,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2736,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>23</v>
@@ -2745,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2756,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -2765,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2777,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2789,7 +2786,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2800,7 +2797,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2811,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2822,7 +2819,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2833,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2844,7 +2841,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2855,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>32</v>
@@ -2864,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2875,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2886,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2897,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2955,26 +2952,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3007,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -3016,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3047,7 +3045,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3058,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -3067,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3109,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>181</v>
@@ -3118,7 +3116,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3129,7 +3127,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>182</v>
@@ -3138,7 +3136,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3150,7 +3148,7 @@
         <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3161,7 +3159,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3172,7 +3170,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3183,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>186</v>
@@ -3192,7 +3190,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3203,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>187</v>
@@ -3212,7 +3210,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3223,7 +3221,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>188</v>
@@ -3232,7 +3230,7 @@
         <v>5</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3243,7 +3241,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>189</v>
@@ -3252,7 +3250,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3263,7 +3261,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>190</v>
@@ -3272,7 +3270,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3283,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>191</v>
@@ -3292,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3303,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>192</v>
@@ -3312,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3323,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>193</v>
@@ -3332,7 +3330,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3343,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>194</v>
@@ -3352,7 +3350,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3363,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>195</v>
@@ -3372,7 +3370,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3383,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>196</v>
@@ -3392,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3403,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>197</v>
@@ -3412,7 +3410,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3423,7 +3421,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>198</v>
@@ -3432,7 +3430,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3443,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>199</v>
@@ -3452,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3463,7 +3461,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>200</v>
@@ -3472,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3483,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>201</v>
@@ -3492,7 +3490,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3503,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>202</v>
@@ -3512,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3523,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>203</v>
@@ -3532,7 +3530,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3543,7 +3541,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>204</v>
@@ -3552,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3563,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>205</v>
@@ -3572,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3583,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>206</v>
@@ -3592,7 +3590,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3603,7 +3601,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>207</v>
@@ -3612,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3623,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>208</v>
@@ -3632,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3643,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>209</v>
@@ -3652,7 +3650,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3663,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>210</v>
@@ -3672,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3683,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>211</v>
@@ -3692,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3703,7 +3701,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>212</v>
@@ -3712,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3723,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>213</v>
@@ -3732,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3743,7 +3741,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>214</v>
@@ -3752,7 +3750,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3763,7 +3761,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>215</v>
@@ -3772,7 +3770,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3783,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>216</v>
@@ -3792,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3803,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>217</v>
@@ -3812,7 +3810,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3823,7 +3821,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>218</v>
@@ -3832,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3843,7 +3841,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>219</v>
@@ -3852,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3863,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>220</v>
@@ -3872,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3883,7 +3881,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>221</v>
@@ -3892,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3903,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>222</v>
@@ -3912,7 +3910,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3923,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>223</v>
@@ -3932,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3943,7 +3941,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3954,7 +3952,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>225</v>
@@ -3963,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3974,7 +3972,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>226</v>
@@ -3983,7 +3981,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3994,7 +3992,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>227</v>
@@ -4003,7 +4001,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4014,7 +4012,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>228</v>
@@ -4023,7 +4021,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4034,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>229</v>
@@ -4043,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4054,7 +4052,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>230</v>
@@ -4063,7 +4061,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4074,7 +4072,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>231</v>
@@ -4083,7 +4081,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4094,7 +4092,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>232</v>
@@ -4103,7 +4101,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4114,7 +4112,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>233</v>
@@ -4123,7 +4121,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4134,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4145,7 +4143,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>235</v>
@@ -4154,7 +4152,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4165,7 +4163,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>236</v>
@@ -4174,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4185,7 +4183,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>237</v>
@@ -4194,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4205,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>238</v>
@@ -4214,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4225,7 +4223,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>239</v>
@@ -4234,7 +4232,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4245,7 +4243,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>240</v>
@@ -4254,7 +4252,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4265,7 +4263,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>241</v>
@@ -4274,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4285,7 +4283,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>242</v>
@@ -4294,7 +4292,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4305,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>243</v>
@@ -4314,7 +4312,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4325,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>244</v>
@@ -4334,7 +4332,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4343,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>245</v>
@@ -4354,7 +4352,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4365,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>246</v>
@@ -4374,7 +4372,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4386,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4397,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>248</v>
@@ -4406,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4417,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>249</v>
@@ -4426,7 +4424,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4437,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>250</v>
@@ -4446,7 +4444,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4457,7 +4455,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4468,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4479,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -4490,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>254</v>
@@ -4499,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4510,7 +4508,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4521,7 +4519,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>256</v>
@@ -4530,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4541,7 +4539,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>257</v>
@@ -4550,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4561,7 +4559,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>258</v>
@@ -4570,7 +4568,7 @@
         <v>1</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4581,7 +4579,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>259</v>
@@ -4590,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4601,7 +4599,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>260</v>
@@ -4610,7 +4608,7 @@
         <v>1</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4621,7 +4619,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>261</v>
@@ -4630,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4641,7 +4639,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>262</v>
@@ -4650,7 +4648,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4661,7 +4659,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>263</v>
@@ -4670,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4681,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>264</v>
@@ -4690,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4702,7 +4700,7 @@
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4714,7 +4712,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4725,7 +4723,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4736,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4747,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>269</v>
@@ -4756,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4767,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>270</v>
@@ -4776,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4787,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>271</v>
@@ -4796,7 +4794,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>486</v>
+        <v>622</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4807,7 +4805,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>272</v>
@@ -4816,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>488</v>
+        <v>623</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4827,7 +4825,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>273</v>
@@ -4836,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4847,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>274</v>
@@ -4856,7 +4854,7 @@
         <v>1</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4867,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>275</v>
@@ -4876,7 +4874,7 @@
         <v>1</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4887,7 +4885,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>276</v>
@@ -4896,7 +4894,7 @@
         <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4907,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>277</v>
@@ -4916,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4927,7 +4925,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>278</v>
@@ -4936,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4947,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>279</v>
@@ -4956,7 +4954,7 @@
         <v>1</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -4967,7 +4965,7 @@
         <v>1</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>280</v>
@@ -4976,7 +4974,7 @@
         <v>1</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4987,7 +4985,7 @@
         <v>1</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>281</v>
@@ -4996,7 +4994,7 @@
         <v>1</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5007,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>282</v>
@@ -5016,7 +5014,7 @@
         <v>1</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5027,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5038,7 +5036,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -5050,7 +5048,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>283</v>
@@ -5059,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5070,7 +5068,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>284</v>
@@ -5079,7 +5077,7 @@
         <v>1</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5090,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>285</v>
@@ -5099,7 +5097,7 @@
         <v>1</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5110,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>286</v>
@@ -5119,7 +5117,7 @@
         <v>1</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -5130,7 +5128,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>287</v>
@@ -5139,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5151,7 +5149,7 @@
         <v>1</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5162,7 +5160,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>289</v>
@@ -5171,7 +5169,7 @@
         <v>1</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5182,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>290</v>
@@ -5191,7 +5189,7 @@
         <v>1</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5202,7 +5200,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>291</v>
@@ -5211,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5222,7 +5220,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5233,7 +5231,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>292</v>
@@ -5242,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -5253,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>293</v>
@@ -5262,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5273,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>294</v>
@@ -5282,7 +5280,7 @@
         <v>1</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5293,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5304,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>296</v>
@@ -5313,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5325,7 +5323,7 @@
         <v>1</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5337,7 +5335,7 @@
         <v>1</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5348,7 +5346,7 @@
         <v>1</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5360,7 +5358,7 @@
         <v>1</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5371,7 +5369,7 @@
         <v>1</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5383,7 +5381,7 @@
         <v>1</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5394,7 +5392,7 @@
         <v>1</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>303</v>
@@ -5403,7 +5401,7 @@
         <v>1</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5414,7 +5412,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>304</v>
@@ -5423,7 +5421,7 @@
         <v>1</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5434,7 +5432,7 @@
         <v>1</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>305</v>
@@ -5443,7 +5441,7 @@
         <v>1</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5454,7 +5452,7 @@
         <v>1</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>306</v>
@@ -5463,7 +5461,7 @@
         <v>1</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5474,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>307</v>
@@ -5483,7 +5481,7 @@
         <v>1</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5494,7 +5492,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>308</v>
@@ -5503,7 +5501,7 @@
         <v>1</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5514,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>309</v>
@@ -5523,7 +5521,7 @@
         <v>1</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5535,7 +5533,7 @@
         <v>1</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5547,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5559,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5571,7 +5569,7 @@
         <v>1</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5582,7 +5580,7 @@
         <v>1</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>314</v>
@@ -5591,7 +5589,7 @@
         <v>1</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5602,7 +5600,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>315</v>
@@ -5611,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -5622,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>316</v>
@@ -5631,7 +5629,7 @@
         <v>1</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5642,7 +5640,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>317</v>
@@ -5651,7 +5649,7 @@
         <v>1</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5662,7 +5660,7 @@
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>318</v>
@@ -5671,7 +5669,7 @@
         <v>1</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5682,7 +5680,7 @@
         <v>1</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>319</v>
@@ -5691,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5702,7 +5700,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>320</v>
@@ -5711,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5722,7 +5720,7 @@
         <v>1</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>321</v>
@@ -5731,7 +5729,7 @@
         <v>1</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5743,7 +5741,7 @@
         <v>5</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5755,7 +5753,7 @@
         <v>5</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5767,7 +5765,7 @@
         <v>5</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5779,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5790,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5801,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>327</v>
@@ -5810,7 +5808,7 @@
         <v>1</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5821,7 +5819,7 @@
         <v>1</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>328</v>
@@ -5830,7 +5828,7 @@
         <v>1</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5842,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5853,7 +5851,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>330</v>
@@ -5862,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5873,7 +5871,7 @@
         <v>1</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>331</v>
@@ -5882,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5893,7 +5891,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>332</v>
@@ -5902,7 +5900,7 @@
         <v>1</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5913,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>333</v>
@@ -5922,7 +5920,7 @@
         <v>1</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5933,7 +5931,7 @@
         <v>1</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>334</v>
@@ -5942,7 +5940,7 @@
         <v>1</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -5953,7 +5951,7 @@
         <v>1</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>335</v>
@@ -5962,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5973,7 +5971,7 @@
         <v>1</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>336</v>
@@ -5982,7 +5980,7 @@
         <v>1</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5993,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>337</v>
@@ -6002,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6013,7 +6011,7 @@
         <v>1</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6024,7 +6022,7 @@
         <v>1</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>339</v>
@@ -6033,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6044,7 +6042,7 @@
         <v>1</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>340</v>
@@ -6053,7 +6051,7 @@
         <v>1</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6064,7 +6062,7 @@
         <v>1</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>341</v>
@@ -6073,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6084,7 +6082,7 @@
         <v>1</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>342</v>
@@ -6093,7 +6091,7 @@
         <v>1</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6104,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>343</v>
@@ -6113,7 +6111,7 @@
         <v>1</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6125,7 +6123,7 @@
         <v>1</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6136,7 +6134,7 @@
         <v>1</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>345</v>
@@ -6145,7 +6143,7 @@
         <v>1</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6157,7 +6155,7 @@
         <v>1</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6168,7 +6166,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>347</v>
@@ -6177,7 +6175,7 @@
         <v>1</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6188,7 +6186,7 @@
         <v>1</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>348</v>
@@ -6197,7 +6195,7 @@
         <v>1</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6208,7 +6206,7 @@
         <v>1</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>349</v>
@@ -6217,7 +6215,7 @@
         <v>1</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6228,7 +6226,7 @@
         <v>1</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6239,7 +6237,7 @@
         <v>1</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>350</v>
@@ -6248,7 +6246,7 @@
         <v>1</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6259,7 +6257,7 @@
         <v>1</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>351</v>
@@ -6268,7 +6266,7 @@
         <v>1</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -6279,7 +6277,7 @@
         <v>1</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>352</v>
@@ -6288,7 +6286,7 @@
         <v>1</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6299,7 +6297,7 @@
         <v>1</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6310,7 +6308,7 @@
         <v>1</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>354</v>
@@ -6319,7 +6317,7 @@
         <v>1</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6330,7 +6328,7 @@
         <v>1</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>355</v>
@@ -6339,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6350,7 +6348,7 @@
         <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>356</v>
@@ -6359,7 +6357,7 @@
         <v>1</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6370,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>357</v>
@@ -6379,7 +6377,7 @@
         <v>1</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6390,7 +6388,7 @@
         <v>1</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>358</v>
@@ -6399,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6411,7 +6409,7 @@
         <v>1</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="193" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6423,7 +6421,7 @@
         <v>1</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="194" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6435,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="195" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6447,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="196" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6459,7 +6457,7 @@
         <v>1</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="197" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6471,7 +6469,7 @@
         <v>1</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="198" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6483,7 +6481,7 @@
         <v>1</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="199" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -6495,7 +6493,7 @@
         <v>1</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.3">
@@ -6544,9 +6542,10 @@
       <c r="C214" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C199">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="notEqual">

</xml_diff>